<commit_message>
📊 Price update for 2026-02-07
✅ Products with price data: 44
⚠️ Out of stock / Failed: 16
⏭️ Skipped (already updated): 0
📊 Total tracked: 60
📈 Success rate: 73%

Scraped at: 2026-02-07
</commit_message>
<xml_diff>
--- a/items/آینه بغل پراید.xlsx
+++ b/items/آینه بغل پراید.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>2025-11-21</t>
+  </si>
+  <si>
+    <t>2026-02-07</t>
+  </si>
+  <si>
+    <t>530000</t>
   </si>
 </sst>
 </file>
@@ -528,7 +534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1049,6 +1055,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>